<commit_message>
Calibrates off-grid H2 capacity shares against Hydrogen Europe projections
</commit_message>
<xml_diff>
--- a/InputData/elec/GHESLE/Green Hydrogen Electricity Supply Logit Exponent.xlsx
+++ b/InputData/elec/GHESLE/Green Hydrogen Electricity Supply Logit Exponent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\GHESLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\GHESLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F6D1AD-05AB-45C8-A56D-A62CCF42C249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BDE776-8B8B-4E1C-9A29-A9216736E8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30120" yWindow="1590" windowWidth="21870" windowHeight="12525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -81,7 +81,7 @@
     <numFmt numFmtId="164" formatCode="###0.00_)"/>
     <numFmt numFmtId="165" formatCode="#,##0_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1150,21 +1150,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1172,47 +1172,47 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
     </row>
   </sheetData>
@@ -1228,27 +1228,27 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-200</v>
+        <v>-100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>